<commit_message>
[Update] add logic split file and create queue job
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_advanced_batch_import/exel/test_import.xlsx
+++ b/addons/custom/forlife_advanced_batch_import/exel/test_import.xlsx
@@ -2960,11 +2960,11 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.3"/>
@@ -26186,7 +26186,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="120.77"/>

</xml_diff>

<commit_message>
[New Feature] Done create module for advanced import
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_advanced_batch_import/exel/test_import.xlsx
+++ b/addons/custom/forlife_advanced_batch_import/exel/test_import.xlsx
@@ -2960,11 +2960,11 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B29" activeCellId="0" sqref="B29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A113" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E136" activeCellId="0" sqref="E136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="45.3"/>
@@ -4772,12 +4772,12 @@
       <c r="Z35" s="3"/>
       <c r="AA35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B36" s="3" t="n">
-        <v>-262</v>
+        <v>1</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="3" t="s">
@@ -4819,12 +4819,12 @@
       <c r="Z36" s="3"/>
       <c r="AA36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B37" s="3" t="n">
-        <v>-261</v>
+        <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>31</v>
@@ -4877,7 +4877,7 @@
         <v>123</v>
       </c>
       <c r="B38" s="3" t="n">
-        <v>-260</v>
+        <v>1</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="3" t="s">
@@ -4925,12 +4925,12 @@
       <c r="Z38" s="3"/>
       <c r="AA38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B39" s="3" t="n">
-        <v>-259</v>
+        <v>1</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="3" t="s">
@@ -4972,12 +4972,12 @@
       <c r="Z39" s="3"/>
       <c r="AA39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>129</v>
       </c>
       <c r="B40" s="3" t="n">
-        <v>-258</v>
+        <v>1</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>31</v>
@@ -5030,7 +5030,7 @@
         <v>131</v>
       </c>
       <c r="B41" s="3" t="n">
-        <v>-257</v>
+        <v>1</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="3" t="s">
@@ -5078,12 +5078,12 @@
       <c r="Z41" s="3"/>
       <c r="AA41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>135</v>
       </c>
       <c r="B42" s="3" t="n">
-        <v>-256</v>
+        <v>1</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="3" t="s">
@@ -5125,12 +5125,12 @@
       <c r="Z42" s="3"/>
       <c r="AA42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B43" s="3" t="n">
-        <v>-255</v>
+        <v>1</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>31</v>
@@ -5183,7 +5183,7 @@
         <v>139</v>
       </c>
       <c r="B44" s="3" t="n">
-        <v>-254</v>
+        <v>1</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="3" t="s">
@@ -5231,12 +5231,12 @@
       <c r="Z44" s="3"/>
       <c r="AA44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
         <v>143</v>
       </c>
       <c r="B45" s="3" t="n">
-        <v>-253</v>
+        <v>1</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="3" t="s">
@@ -5278,12 +5278,12 @@
       <c r="Z45" s="3"/>
       <c r="AA45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B46" s="3" t="n">
-        <v>-252</v>
+        <v>1</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>31</v>
@@ -5336,7 +5336,7 @@
         <v>147</v>
       </c>
       <c r="B47" s="3" t="n">
-        <v>-251</v>
+        <v>1</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="3" t="s">
@@ -5384,12 +5384,12 @@
       <c r="Z47" s="3"/>
       <c r="AA47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
         <v>151</v>
       </c>
       <c r="B48" s="3" t="n">
-        <v>-250</v>
+        <v>1</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="3" t="s">
@@ -5431,12 +5431,12 @@
       <c r="Z48" s="3"/>
       <c r="AA48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
         <v>153</v>
       </c>
       <c r="B49" s="3" t="n">
-        <v>-249</v>
+        <v>1</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>31</v>
@@ -5489,7 +5489,7 @@
         <v>155</v>
       </c>
       <c r="B50" s="3" t="n">
-        <v>-248</v>
+        <v>1</v>
       </c>
       <c r="C50" s="4"/>
       <c r="D50" s="3" t="s">
@@ -5537,12 +5537,12 @@
       <c r="Z50" s="3"/>
       <c r="AA50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
         <v>159</v>
       </c>
       <c r="B51" s="3" t="n">
-        <v>-247</v>
+        <v>1</v>
       </c>
       <c r="C51" s="4"/>
       <c r="D51" s="3" t="s">
@@ -5584,12 +5584,12 @@
       <c r="Z51" s="3"/>
       <c r="AA51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
         <v>161</v>
       </c>
       <c r="B52" s="3" t="n">
-        <v>-246</v>
+        <v>1</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>31</v>
@@ -5642,7 +5642,7 @@
         <v>163</v>
       </c>
       <c r="B53" s="3" t="n">
-        <v>-245</v>
+        <v>1</v>
       </c>
       <c r="C53" s="4"/>
       <c r="D53" s="3" t="s">
@@ -5690,12 +5690,12 @@
       <c r="Z53" s="3"/>
       <c r="AA53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
         <v>167</v>
       </c>
       <c r="B54" s="3" t="n">
-        <v>-244</v>
+        <v>1</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="3" t="s">
@@ -5737,12 +5737,12 @@
       <c r="Z54" s="3"/>
       <c r="AA54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
         <v>169</v>
       </c>
       <c r="B55" s="3" t="n">
-        <v>-243</v>
+        <v>1</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>31</v>
@@ -5795,7 +5795,7 @@
         <v>171</v>
       </c>
       <c r="B56" s="3" t="n">
-        <v>-242</v>
+        <v>1</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="3" t="s">
@@ -5843,12 +5843,12 @@
       <c r="Z56" s="3"/>
       <c r="AA56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
         <v>175</v>
       </c>
       <c r="B57" s="3" t="n">
-        <v>-241</v>
+        <v>1</v>
       </c>
       <c r="C57" s="4"/>
       <c r="D57" s="3" t="s">
@@ -5890,12 +5890,12 @@
       <c r="Z57" s="3"/>
       <c r="AA57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
         <v>177</v>
       </c>
       <c r="B58" s="3" t="n">
-        <v>-240</v>
+        <v>1</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>31</v>
@@ -5948,7 +5948,7 @@
         <v>179</v>
       </c>
       <c r="B59" s="3" t="n">
-        <v>-239</v>
+        <v>1</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="3" t="s">
@@ -5996,12 +5996,12 @@
       <c r="Z59" s="3"/>
       <c r="AA59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
         <v>183</v>
       </c>
       <c r="B60" s="3" t="n">
-        <v>-238</v>
+        <v>1</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="3" t="s">
@@ -6043,12 +6043,12 @@
       <c r="Z60" s="3"/>
       <c r="AA60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B61" s="3" t="n">
-        <v>-237</v>
+        <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>31</v>
@@ -6101,7 +6101,7 @@
         <v>187</v>
       </c>
       <c r="B62" s="3" t="n">
-        <v>-236</v>
+        <v>1</v>
       </c>
       <c r="C62" s="4"/>
       <c r="D62" s="3" t="s">
@@ -6149,12 +6149,12 @@
       <c r="Z62" s="3"/>
       <c r="AA62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B63" s="3" t="n">
-        <v>-235</v>
+        <v>1</v>
       </c>
       <c r="C63" s="4"/>
       <c r="D63" s="3" t="s">
@@ -6196,12 +6196,12 @@
       <c r="Z63" s="3"/>
       <c r="AA63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
         <v>193</v>
       </c>
       <c r="B64" s="3" t="n">
-        <v>-234</v>
+        <v>1</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>31</v>
@@ -6254,7 +6254,7 @@
         <v>195</v>
       </c>
       <c r="B65" s="3" t="n">
-        <v>-233</v>
+        <v>1</v>
       </c>
       <c r="C65" s="4"/>
       <c r="D65" s="3" t="s">
@@ -6302,12 +6302,12 @@
       <c r="Z65" s="3"/>
       <c r="AA65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
         <v>199</v>
       </c>
       <c r="B66" s="3" t="n">
-        <v>-232</v>
+        <v>1</v>
       </c>
       <c r="C66" s="4"/>
       <c r="D66" s="3" t="s">
@@ -6349,12 +6349,12 @@
       <c r="Z66" s="3"/>
       <c r="AA66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
         <v>201</v>
       </c>
       <c r="B67" s="3" t="n">
-        <v>-231</v>
+        <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>31</v>
@@ -6407,7 +6407,7 @@
         <v>203</v>
       </c>
       <c r="B68" s="3" t="n">
-        <v>-230</v>
+        <v>1</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="3" t="s">
@@ -6455,12 +6455,12 @@
       <c r="Z68" s="3"/>
       <c r="AA68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B69" s="3" t="n">
-        <v>-229</v>
+        <v>1</v>
       </c>
       <c r="C69" s="4"/>
       <c r="D69" s="3" t="s">
@@ -6502,12 +6502,12 @@
       <c r="Z69" s="3"/>
       <c r="AA69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
         <v>209</v>
       </c>
       <c r="B70" s="3" t="n">
-        <v>-228</v>
+        <v>1</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>31</v>
@@ -6560,7 +6560,7 @@
         <v>211</v>
       </c>
       <c r="B71" s="3" t="n">
-        <v>-227</v>
+        <v>1</v>
       </c>
       <c r="C71" s="4"/>
       <c r="D71" s="3" t="s">
@@ -6608,12 +6608,12 @@
       <c r="Z71" s="3"/>
       <c r="AA71" s="3"/>
     </row>
-    <row r="72" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
         <v>215</v>
       </c>
       <c r="B72" s="3" t="n">
-        <v>-226</v>
+        <v>1</v>
       </c>
       <c r="C72" s="4"/>
       <c r="D72" s="3" t="s">
@@ -6655,12 +6655,12 @@
       <c r="Z72" s="3"/>
       <c r="AA72" s="3"/>
     </row>
-    <row r="73" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
         <v>217</v>
       </c>
       <c r="B73" s="3" t="n">
-        <v>-225</v>
+        <v>1</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>31</v>
@@ -6713,7 +6713,7 @@
         <v>219</v>
       </c>
       <c r="B74" s="3" t="n">
-        <v>-224</v>
+        <v>1</v>
       </c>
       <c r="C74" s="4"/>
       <c r="D74" s="3" t="s">
@@ -6761,12 +6761,12 @@
       <c r="Z74" s="3"/>
       <c r="AA74" s="3"/>
     </row>
-    <row r="75" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
         <v>223</v>
       </c>
       <c r="B75" s="3" t="n">
-        <v>-223</v>
+        <v>1</v>
       </c>
       <c r="C75" s="4"/>
       <c r="D75" s="3" t="s">
@@ -6808,12 +6808,12 @@
       <c r="Z75" s="3"/>
       <c r="AA75" s="3"/>
     </row>
-    <row r="76" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
         <v>225</v>
       </c>
       <c r="B76" s="3" t="n">
-        <v>-222</v>
+        <v>1</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>31</v>
@@ -6866,7 +6866,7 @@
         <v>227</v>
       </c>
       <c r="B77" s="3" t="n">
-        <v>-221</v>
+        <v>1</v>
       </c>
       <c r="C77" s="4"/>
       <c r="D77" s="3" t="s">
@@ -6914,12 +6914,12 @@
       <c r="Z77" s="3"/>
       <c r="AA77" s="3"/>
     </row>
-    <row r="78" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
         <v>231</v>
       </c>
       <c r="B78" s="3" t="n">
-        <v>-220</v>
+        <v>1</v>
       </c>
       <c r="C78" s="4"/>
       <c r="D78" s="3" t="s">
@@ -6961,12 +6961,12 @@
       <c r="Z78" s="3"/>
       <c r="AA78" s="3"/>
     </row>
-    <row r="79" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
         <v>233</v>
       </c>
       <c r="B79" s="3" t="n">
-        <v>-219</v>
+        <v>1</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>31</v>
@@ -7019,7 +7019,7 @@
         <v>235</v>
       </c>
       <c r="B80" s="3" t="n">
-        <v>-218</v>
+        <v>1</v>
       </c>
       <c r="C80" s="4"/>
       <c r="D80" s="3" t="s">
@@ -7067,12 +7067,12 @@
       <c r="Z80" s="3"/>
       <c r="AA80" s="3"/>
     </row>
-    <row r="81" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
         <v>239</v>
       </c>
       <c r="B81" s="3" t="n">
-        <v>-217</v>
+        <v>1</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="3" t="s">
@@ -7114,12 +7114,12 @@
       <c r="Z81" s="3"/>
       <c r="AA81" s="3"/>
     </row>
-    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
         <v>241</v>
       </c>
       <c r="B82" s="3" t="n">
-        <v>-216</v>
+        <v>1</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>31</v>
@@ -7172,7 +7172,7 @@
         <v>243</v>
       </c>
       <c r="B83" s="3" t="n">
-        <v>-215</v>
+        <v>1</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="3" t="s">
@@ -7220,12 +7220,12 @@
       <c r="Z83" s="3"/>
       <c r="AA83" s="3"/>
     </row>
-    <row r="84" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B84" s="3" t="n">
-        <v>-214</v>
+        <v>1</v>
       </c>
       <c r="C84" s="4"/>
       <c r="D84" s="3" t="s">
@@ -7267,12 +7267,12 @@
       <c r="Z84" s="3"/>
       <c r="AA84" s="3"/>
     </row>
-    <row r="85" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
         <v>249</v>
       </c>
       <c r="B85" s="3" t="n">
-        <v>-213</v>
+        <v>1</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>31</v>
@@ -7325,7 +7325,7 @@
         <v>251</v>
       </c>
       <c r="B86" s="3" t="n">
-        <v>-212</v>
+        <v>1</v>
       </c>
       <c r="C86" s="4"/>
       <c r="D86" s="3" t="s">
@@ -7373,12 +7373,12 @@
       <c r="Z86" s="3"/>
       <c r="AA86" s="3"/>
     </row>
-    <row r="87" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
         <v>255</v>
       </c>
       <c r="B87" s="3" t="n">
-        <v>-211</v>
+        <v>1</v>
       </c>
       <c r="C87" s="4"/>
       <c r="D87" s="3" t="s">
@@ -7420,12 +7420,12 @@
       <c r="Z87" s="3"/>
       <c r="AA87" s="3"/>
     </row>
-    <row r="88" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
         <v>257</v>
       </c>
       <c r="B88" s="3" t="n">
-        <v>-210</v>
+        <v>1</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>31</v>
@@ -7478,7 +7478,7 @@
         <v>259</v>
       </c>
       <c r="B89" s="3" t="n">
-        <v>-209</v>
+        <v>1</v>
       </c>
       <c r="C89" s="4"/>
       <c r="D89" s="3" t="s">
@@ -7526,12 +7526,12 @@
       <c r="Z89" s="3"/>
       <c r="AA89" s="3"/>
     </row>
-    <row r="90" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
         <v>263</v>
       </c>
       <c r="B90" s="3" t="n">
-        <v>-208</v>
+        <v>1</v>
       </c>
       <c r="C90" s="4"/>
       <c r="D90" s="3" t="s">
@@ -7573,12 +7573,12 @@
       <c r="Z90" s="3"/>
       <c r="AA90" s="3"/>
     </row>
-    <row r="91" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B91" s="3" t="n">
-        <v>-207</v>
+        <v>1</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>31</v>
@@ -7631,7 +7631,7 @@
         <v>267</v>
       </c>
       <c r="B92" s="3" t="n">
-        <v>-206</v>
+        <v>1</v>
       </c>
       <c r="C92" s="4"/>
       <c r="D92" s="3" t="s">
@@ -7679,12 +7679,12 @@
       <c r="Z92" s="3"/>
       <c r="AA92" s="3"/>
     </row>
-    <row r="93" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B93" s="3" t="n">
-        <v>-205</v>
+        <v>1</v>
       </c>
       <c r="C93" s="4"/>
       <c r="D93" s="3" t="s">
@@ -7726,12 +7726,12 @@
       <c r="Z93" s="3"/>
       <c r="AA93" s="3"/>
     </row>
-    <row r="94" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B94" s="3" t="n">
-        <v>-204</v>
+        <v>1</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>31</v>
@@ -7784,7 +7784,7 @@
         <v>275</v>
       </c>
       <c r="B95" s="3" t="n">
-        <v>-203</v>
+        <v>1</v>
       </c>
       <c r="C95" s="4"/>
       <c r="D95" s="3" t="s">
@@ -7832,12 +7832,12 @@
       <c r="Z95" s="3"/>
       <c r="AA95" s="3"/>
     </row>
-    <row r="96" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B96" s="3" t="n">
-        <v>-202</v>
+        <v>1</v>
       </c>
       <c r="C96" s="4"/>
       <c r="D96" s="3" t="s">
@@ -7879,12 +7879,12 @@
       <c r="Z96" s="3"/>
       <c r="AA96" s="3"/>
     </row>
-    <row r="97" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
         <v>281</v>
       </c>
       <c r="B97" s="3" t="n">
-        <v>-201</v>
+        <v>1</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>31</v>
@@ -7937,7 +7937,7 @@
         <v>283</v>
       </c>
       <c r="B98" s="3" t="n">
-        <v>-200</v>
+        <v>1</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="3" t="s">
@@ -7985,12 +7985,12 @@
       <c r="Z98" s="3"/>
       <c r="AA98" s="3"/>
     </row>
-    <row r="99" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
         <v>287</v>
       </c>
       <c r="B99" s="3" t="n">
-        <v>-199</v>
+        <v>1</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="3" t="s">
@@ -8032,12 +8032,12 @@
       <c r="Z99" s="3"/>
       <c r="AA99" s="3"/>
     </row>
-    <row r="100" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
         <v>289</v>
       </c>
       <c r="B100" s="3" t="n">
-        <v>-198</v>
+        <v>1</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>31</v>
@@ -8090,7 +8090,7 @@
         <v>291</v>
       </c>
       <c r="B101" s="3" t="n">
-        <v>-197</v>
+        <v>1</v>
       </c>
       <c r="C101" s="4"/>
       <c r="D101" s="3" t="s">
@@ -8138,12 +8138,12 @@
       <c r="Z101" s="3"/>
       <c r="AA101" s="3"/>
     </row>
-    <row r="102" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
         <v>295</v>
       </c>
       <c r="B102" s="3" t="n">
-        <v>-196</v>
+        <v>1</v>
       </c>
       <c r="C102" s="4"/>
       <c r="D102" s="3" t="s">
@@ -8185,12 +8185,12 @@
       <c r="Z102" s="3"/>
       <c r="AA102" s="3"/>
     </row>
-    <row r="103" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B103" s="3" t="n">
-        <v>-195</v>
+        <v>1</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>31</v>
@@ -8243,7 +8243,7 @@
         <v>299</v>
       </c>
       <c r="B104" s="3" t="n">
-        <v>-194</v>
+        <v>1</v>
       </c>
       <c r="C104" s="4"/>
       <c r="D104" s="3" t="s">
@@ -8291,12 +8291,12 @@
       <c r="Z104" s="3"/>
       <c r="AA104" s="3"/>
     </row>
-    <row r="105" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
         <v>303</v>
       </c>
       <c r="B105" s="3" t="n">
-        <v>-193</v>
+        <v>1</v>
       </c>
       <c r="C105" s="4"/>
       <c r="D105" s="3" t="s">
@@ -8338,12 +8338,12 @@
       <c r="Z105" s="3"/>
       <c r="AA105" s="3"/>
     </row>
-    <row r="106" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
         <v>305</v>
       </c>
       <c r="B106" s="3" t="n">
-        <v>-192</v>
+        <v>1</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>31</v>
@@ -8396,7 +8396,7 @@
         <v>307</v>
       </c>
       <c r="B107" s="3" t="n">
-        <v>-191</v>
+        <v>1</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="3" t="s">
@@ -8444,12 +8444,12 @@
       <c r="Z107" s="3"/>
       <c r="AA107" s="3"/>
     </row>
-    <row r="108" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
         <v>311</v>
       </c>
       <c r="B108" s="3" t="n">
-        <v>-190</v>
+        <v>1</v>
       </c>
       <c r="C108" s="4"/>
       <c r="D108" s="3" t="s">
@@ -8491,12 +8491,12 @@
       <c r="Z108" s="3"/>
       <c r="AA108" s="3"/>
     </row>
-    <row r="109" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
         <v>313</v>
       </c>
       <c r="B109" s="3" t="n">
-        <v>-189</v>
+        <v>1</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>31</v>
@@ -8549,7 +8549,7 @@
         <v>315</v>
       </c>
       <c r="B110" s="3" t="n">
-        <v>-188</v>
+        <v>1</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="3" t="s">
@@ -8597,12 +8597,12 @@
       <c r="Z110" s="3"/>
       <c r="AA110" s="3"/>
     </row>
-    <row r="111" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
         <v>319</v>
       </c>
       <c r="B111" s="3" t="n">
-        <v>-187</v>
+        <v>1</v>
       </c>
       <c r="C111" s="4"/>
       <c r="D111" s="3" t="s">
@@ -8644,12 +8644,12 @@
       <c r="Z111" s="3"/>
       <c r="AA111" s="3"/>
     </row>
-    <row r="112" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
         <v>321</v>
       </c>
       <c r="B112" s="3" t="n">
-        <v>-186</v>
+        <v>1</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>31</v>
@@ -8702,7 +8702,7 @@
         <v>323</v>
       </c>
       <c r="B113" s="3" t="n">
-        <v>-185</v>
+        <v>1</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="3" t="s">
@@ -8750,12 +8750,12 @@
       <c r="Z113" s="3"/>
       <c r="AA113" s="3"/>
     </row>
-    <row r="114" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B114" s="3" t="n">
-        <v>-184</v>
+        <v>1</v>
       </c>
       <c r="C114" s="4"/>
       <c r="D114" s="3" t="s">
@@ -8797,12 +8797,12 @@
       <c r="Z114" s="3"/>
       <c r="AA114" s="3"/>
     </row>
-    <row r="115" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
         <v>329</v>
       </c>
       <c r="B115" s="3" t="n">
-        <v>-183</v>
+        <v>1</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>31</v>
@@ -8855,7 +8855,7 @@
         <v>331</v>
       </c>
       <c r="B116" s="3" t="n">
-        <v>-182</v>
+        <v>1</v>
       </c>
       <c r="C116" s="4"/>
       <c r="D116" s="3" t="s">
@@ -8903,12 +8903,12 @@
       <c r="Z116" s="3"/>
       <c r="AA116" s="3"/>
     </row>
-    <row r="117" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
         <v>335</v>
       </c>
       <c r="B117" s="3" t="n">
-        <v>-181</v>
+        <v>1</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="3" t="s">
@@ -8950,12 +8950,12 @@
       <c r="Z117" s="3"/>
       <c r="AA117" s="3"/>
     </row>
-    <row r="118" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
         <v>337</v>
       </c>
       <c r="B118" s="3" t="n">
-        <v>-180</v>
+        <v>1</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>31</v>
@@ -9008,7 +9008,7 @@
         <v>339</v>
       </c>
       <c r="B119" s="3" t="n">
-        <v>-179</v>
+        <v>1</v>
       </c>
       <c r="C119" s="4"/>
       <c r="D119" s="3" t="s">
@@ -9056,12 +9056,12 @@
       <c r="Z119" s="3"/>
       <c r="AA119" s="3"/>
     </row>
-    <row r="120" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
         <v>343</v>
       </c>
       <c r="B120" s="3" t="n">
-        <v>-178</v>
+        <v>1</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="3" t="s">
@@ -9103,12 +9103,12 @@
       <c r="Z120" s="3"/>
       <c r="AA120" s="3"/>
     </row>
-    <row r="121" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
         <v>345</v>
       </c>
       <c r="B121" s="3" t="n">
-        <v>-177</v>
+        <v>1</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>31</v>
@@ -9161,7 +9161,7 @@
         <v>347</v>
       </c>
       <c r="B122" s="3" t="n">
-        <v>-176</v>
+        <v>1</v>
       </c>
       <c r="C122" s="4"/>
       <c r="D122" s="3" t="s">
@@ -9209,12 +9209,12 @@
       <c r="Z122" s="3"/>
       <c r="AA122" s="3"/>
     </row>
-    <row r="123" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
         <v>351</v>
       </c>
       <c r="B123" s="3" t="n">
-        <v>-175</v>
+        <v>1</v>
       </c>
       <c r="C123" s="4"/>
       <c r="D123" s="3" t="s">
@@ -9256,12 +9256,12 @@
       <c r="Z123" s="3"/>
       <c r="AA123" s="3"/>
     </row>
-    <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
         <v>353</v>
       </c>
       <c r="B124" s="3" t="n">
-        <v>-174</v>
+        <v>1</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>31</v>
@@ -9314,7 +9314,7 @@
         <v>355</v>
       </c>
       <c r="B125" s="3" t="n">
-        <v>-173</v>
+        <v>1</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="3" t="s">
@@ -9362,12 +9362,12 @@
       <c r="Z125" s="3"/>
       <c r="AA125" s="3"/>
     </row>
-    <row r="126" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
         <v>359</v>
       </c>
       <c r="B126" s="3" t="n">
-        <v>-172</v>
+        <v>1</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="3" t="s">
@@ -9409,12 +9409,12 @@
       <c r="Z126" s="3"/>
       <c r="AA126" s="3"/>
     </row>
-    <row r="127" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
         <v>361</v>
       </c>
       <c r="B127" s="3" t="n">
-        <v>-171</v>
+        <v>1</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>31</v>
@@ -9467,7 +9467,7 @@
         <v>363</v>
       </c>
       <c r="B128" s="3" t="n">
-        <v>-170</v>
+        <v>1</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="3" t="s">
@@ -9515,12 +9515,12 @@
       <c r="Z128" s="3"/>
       <c r="AA128" s="3"/>
     </row>
-    <row r="129" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
         <v>367</v>
       </c>
       <c r="B129" s="3" t="n">
-        <v>-169</v>
+        <v>1</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="3" t="s">
@@ -9562,12 +9562,12 @@
       <c r="Z129" s="3"/>
       <c r="AA129" s="3"/>
     </row>
-    <row r="130" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
         <v>369</v>
       </c>
       <c r="B130" s="3" t="n">
-        <v>-168</v>
+        <v>1</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>31</v>
@@ -9620,7 +9620,7 @@
         <v>371</v>
       </c>
       <c r="B131" s="3" t="n">
-        <v>-167</v>
+        <v>1</v>
       </c>
       <c r="C131" s="4"/>
       <c r="D131" s="3" t="s">
@@ -9668,12 +9668,12 @@
       <c r="Z131" s="3"/>
       <c r="AA131" s="3"/>
     </row>
-    <row r="132" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
         <v>375</v>
       </c>
       <c r="B132" s="3" t="n">
-        <v>-166</v>
+        <v>1</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="3" t="s">
@@ -9715,12 +9715,12 @@
       <c r="Z132" s="3"/>
       <c r="AA132" s="3"/>
     </row>
-    <row r="133" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
         <v>377</v>
       </c>
       <c r="B133" s="3" t="n">
-        <v>-165</v>
+        <v>1</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>31</v>
@@ -9773,7 +9773,7 @@
         <v>379</v>
       </c>
       <c r="B134" s="3" t="n">
-        <v>-164</v>
+        <v>1</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="3" t="s">
@@ -9821,12 +9821,12 @@
       <c r="Z134" s="3"/>
       <c r="AA134" s="3"/>
     </row>
-    <row r="135" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
         <v>383</v>
       </c>
       <c r="B135" s="3" t="n">
-        <v>-163</v>
+        <v>1</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="3" t="s">
@@ -9868,12 +9868,12 @@
       <c r="Z135" s="3"/>
       <c r="AA135" s="3"/>
     </row>
-    <row r="136" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
         <v>385</v>
       </c>
       <c r="B136" s="3" t="n">
-        <v>-162</v>
+        <v>1</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>31</v>
@@ -9926,7 +9926,7 @@
         <v>387</v>
       </c>
       <c r="B137" s="3" t="n">
-        <v>-161</v>
+        <v>1</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="3" t="s">
@@ -9974,12 +9974,12 @@
       <c r="Z137" s="3"/>
       <c r="AA137" s="3"/>
     </row>
-    <row r="138" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
         <v>391</v>
       </c>
       <c r="B138" s="3" t="n">
-        <v>-160</v>
+        <v>1</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="3" t="s">
@@ -10021,12 +10021,12 @@
       <c r="Z138" s="3"/>
       <c r="AA138" s="3"/>
     </row>
-    <row r="139" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
         <v>393</v>
       </c>
       <c r="B139" s="3" t="n">
-        <v>-159</v>
+        <v>1</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>31</v>
@@ -10079,7 +10079,7 @@
         <v>395</v>
       </c>
       <c r="B140" s="3" t="n">
-        <v>-158</v>
+        <v>1</v>
       </c>
       <c r="C140" s="4"/>
       <c r="D140" s="3" t="s">
@@ -10127,12 +10127,12 @@
       <c r="Z140" s="3"/>
       <c r="AA140" s="3"/>
     </row>
-    <row r="141" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
         <v>399</v>
       </c>
       <c r="B141" s="3" t="n">
-        <v>-157</v>
+        <v>1</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="3" t="s">
@@ -10174,12 +10174,12 @@
       <c r="Z141" s="3"/>
       <c r="AA141" s="3"/>
     </row>
-    <row r="142" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
         <v>401</v>
       </c>
       <c r="B142" s="3" t="n">
-        <v>-156</v>
+        <v>1</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>31</v>
@@ -10232,7 +10232,7 @@
         <v>403</v>
       </c>
       <c r="B143" s="3" t="n">
-        <v>-155</v>
+        <v>1</v>
       </c>
       <c r="C143" s="4"/>
       <c r="D143" s="3" t="s">
@@ -10280,12 +10280,12 @@
       <c r="Z143" s="3"/>
       <c r="AA143" s="3"/>
     </row>
-    <row r="144" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
         <v>407</v>
       </c>
       <c r="B144" s="3" t="n">
-        <v>-154</v>
+        <v>1</v>
       </c>
       <c r="C144" s="4"/>
       <c r="D144" s="3" t="s">
@@ -10327,12 +10327,12 @@
       <c r="Z144" s="3"/>
       <c r="AA144" s="3"/>
     </row>
-    <row r="145" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
         <v>409</v>
       </c>
       <c r="B145" s="3" t="n">
-        <v>-153</v>
+        <v>1</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>31</v>
@@ -10385,7 +10385,7 @@
         <v>411</v>
       </c>
       <c r="B146" s="3" t="n">
-        <v>-152</v>
+        <v>1</v>
       </c>
       <c r="C146" s="4"/>
       <c r="D146" s="3" t="s">
@@ -10433,12 +10433,12 @@
       <c r="Z146" s="3"/>
       <c r="AA146" s="3"/>
     </row>
-    <row r="147" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="s">
         <v>415</v>
       </c>
       <c r="B147" s="3" t="n">
-        <v>-151</v>
+        <v>1</v>
       </c>
       <c r="C147" s="4"/>
       <c r="D147" s="3" t="s">
@@ -10480,12 +10480,12 @@
       <c r="Z147" s="3"/>
       <c r="AA147" s="3"/>
     </row>
-    <row r="148" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="s">
         <v>417</v>
       </c>
       <c r="B148" s="3" t="n">
-        <v>-150</v>
+        <v>1</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>31</v>
@@ -10538,7 +10538,7 @@
         <v>419</v>
       </c>
       <c r="B149" s="3" t="n">
-        <v>-149</v>
+        <v>1</v>
       </c>
       <c r="C149" s="4"/>
       <c r="D149" s="3" t="s">
@@ -10586,12 +10586,12 @@
       <c r="Z149" s="3"/>
       <c r="AA149" s="3"/>
     </row>
-    <row r="150" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="3" t="s">
         <v>423</v>
       </c>
       <c r="B150" s="3" t="n">
-        <v>-148</v>
+        <v>1</v>
       </c>
       <c r="C150" s="4"/>
       <c r="D150" s="3" t="s">
@@ -10633,12 +10633,12 @@
       <c r="Z150" s="3"/>
       <c r="AA150" s="3"/>
     </row>
-    <row r="151" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="3" t="s">
         <v>425</v>
       </c>
       <c r="B151" s="3" t="n">
-        <v>-147</v>
+        <v>1</v>
       </c>
       <c r="C151" s="3" t="s">
         <v>31</v>
@@ -10691,7 +10691,7 @@
         <v>427</v>
       </c>
       <c r="B152" s="3" t="n">
-        <v>-146</v>
+        <v>1</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="3" t="s">
@@ -10739,12 +10739,12 @@
       <c r="Z152" s="3"/>
       <c r="AA152" s="3"/>
     </row>
-    <row r="153" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="3" t="s">
         <v>431</v>
       </c>
       <c r="B153" s="3" t="n">
-        <v>-145</v>
+        <v>1</v>
       </c>
       <c r="C153" s="4"/>
       <c r="D153" s="3" t="s">
@@ -10786,12 +10786,12 @@
       <c r="Z153" s="3"/>
       <c r="AA153" s="3"/>
     </row>
-    <row r="154" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="3" t="s">
         <v>433</v>
       </c>
       <c r="B154" s="3" t="n">
-        <v>-144</v>
+        <v>1</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>31</v>
@@ -10844,7 +10844,7 @@
         <v>435</v>
       </c>
       <c r="B155" s="3" t="n">
-        <v>-143</v>
+        <v>1</v>
       </c>
       <c r="C155" s="4"/>
       <c r="D155" s="3" t="s">
@@ -10892,12 +10892,12 @@
       <c r="Z155" s="3"/>
       <c r="AA155" s="3"/>
     </row>
-    <row r="156" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="3" t="s">
         <v>439</v>
       </c>
       <c r="B156" s="3" t="n">
-        <v>-142</v>
+        <v>1</v>
       </c>
       <c r="C156" s="4"/>
       <c r="D156" s="3" t="s">
@@ -10939,12 +10939,12 @@
       <c r="Z156" s="3"/>
       <c r="AA156" s="3"/>
     </row>
-    <row r="157" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="3" t="s">
         <v>441</v>
       </c>
       <c r="B157" s="3" t="n">
-        <v>-141</v>
+        <v>1</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>31</v>
@@ -26186,7 +26186,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="120.77"/>

</xml_diff>